<commit_message>
add zyx and hzj
</commit_message>
<xml_diff>
--- a/Data/全部数据/原始excel/混合调节(K=1~2)/k=1.0/k=1.0所有概率值.xlsx
+++ b/Data/全部数据/原始excel/混合调节(K=1~2)/k=1.0/k=1.0所有概率值.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="10290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>hzj-混合调节_20170512_112118_ASIC_EEG</t>
   </si>
@@ -57,6 +57,30 @@
   </si>
   <si>
     <t>wzq-混合调节_20170512_115256_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>hzj-混合调节_20170516_152754_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>hzj-混合调节_20170518_134207_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>hzj-混合调节_20170519_135415_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>zyx-混合调节_20170516_111228_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>zyx-混合调节_20170517_110944_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>zyx-混合调节_20170518_112337_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>zyx-混合调节_20170519_124954_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>zyx-混合调节_20170522_111557_ASIC_EEG</t>
   </si>
 </sst>
 </file>
@@ -386,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K3"/>
+      <selection sqref="A1:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,8 +452,32 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.65979381443298968</v>
       </c>
@@ -463,8 +511,32 @@
       <c r="K2">
         <v>0.6901408450704225</v>
       </c>
+      <c r="L2">
+        <v>0.5625</v>
+      </c>
+      <c r="M2">
+        <v>0.59450171821305842</v>
+      </c>
+      <c r="N2">
+        <v>0.62172284644194753</v>
+      </c>
+      <c r="O2">
+        <v>0.59935897435897434</v>
+      </c>
+      <c r="P2">
+        <v>0.70192307692307687</v>
+      </c>
+      <c r="Q2">
+        <v>0.69255663430420711</v>
+      </c>
+      <c r="R2">
+        <v>0.6064516129032258</v>
+      </c>
+      <c r="S2">
+        <v>0.65776699029126218</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.66246056782334384</v>
       </c>
@@ -497,6 +569,30 @@
       </c>
       <c r="K3">
         <v>0.63973063973063971</v>
+      </c>
+      <c r="L3">
+        <v>0.53479853479853479</v>
+      </c>
+      <c r="M3">
+        <v>0.57741935483870965</v>
+      </c>
+      <c r="N3">
+        <v>0.58608058608058611</v>
+      </c>
+      <c r="O3">
+        <v>0.57857142857142851</v>
+      </c>
+      <c r="P3">
+        <v>0.65363128491620115</v>
+      </c>
+      <c r="Q3">
+        <v>0.60824742268041243</v>
+      </c>
+      <c r="R3">
+        <v>0.60738255033557054</v>
+      </c>
+      <c r="S3">
+        <v>0.63203463203463206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>